<commit_message>
better node and unit hover tooltip
</commit_message>
<xml_diff>
--- a/contents/battle/battle_1/battle_1.xlsx
+++ b/contents/battle/battle_1/battle_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imanol-KS53\Documents\Imanol\Github_projects\InteractiveBook\contents\battle\battle_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71465F13-0C31-4006-A1FA-579DC0CD45EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3A6C05-7974-406B-AB96-DE138733BF67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,27 +102,6 @@
     <t>other</t>
   </si>
   <si>
-    <t>b1</t>
-  </si>
-  <si>
-    <t>b2</t>
-  </si>
-  <si>
-    <t>b3</t>
-  </si>
-  <si>
-    <t>side</t>
-  </si>
-  <si>
-    <t>h1</t>
-  </si>
-  <si>
-    <t>h2</t>
-  </si>
-  <si>
-    <t>h3</t>
-  </si>
-  <si>
     <t>Goblin Warrior</t>
   </si>
   <si>
@@ -135,9 +114,6 @@
     <t>Dwarf Archer</t>
   </si>
   <si>
-    <t>h4</t>
-  </si>
-  <si>
     <t>from</t>
   </si>
   <si>
@@ -150,12 +126,6 @@
     <t>archer</t>
   </si>
   <si>
-    <t>b1,b2</t>
-  </si>
-  <si>
-    <t>b2,b3</t>
-  </si>
-  <si>
     <t>all</t>
   </si>
   <si>
@@ -208,6 +178,36 @@
   </si>
   <si>
     <t>cavalry</t>
+  </si>
+  <si>
+    <t>bridge_1</t>
+  </si>
+  <si>
+    <t>hill_1</t>
+  </si>
+  <si>
+    <t>hill_2</t>
+  </si>
+  <si>
+    <t>hill_3</t>
+  </si>
+  <si>
+    <t>bridge_2</t>
+  </si>
+  <si>
+    <t>bridge_3</t>
+  </si>
+  <si>
+    <t>bridge_1,bridge_2</t>
+  </si>
+  <si>
+    <t>bridge_2,bridge_3</t>
+  </si>
+  <si>
+    <t>north_side</t>
+  </si>
+  <si>
+    <t>south_side</t>
   </si>
 </sst>
 </file>
@@ -617,7 +617,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +668,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>9</v>
@@ -688,7 +688,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>9</v>
@@ -708,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>9</v>
@@ -728,7 +728,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>9</v>
@@ -748,7 +748,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>9</v>
@@ -768,10 +768,10 @@
         <v>0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -788,10 +788,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -808,10 +808,10 @@
         <v>0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -828,10 +828,10 @@
         <v>0</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -848,10 +848,10 @@
         <v>0</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -868,10 +868,10 @@
         <v>0</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -888,10 +888,10 @@
         <v>1</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>9</v>
@@ -911,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>9</v>
@@ -931,10 +931,10 @@
         <v>1</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>9</v>
@@ -954,7 +954,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -971,10 +971,10 @@
         <v>2</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>9</v>
@@ -994,10 +994,10 @@
         <v>2</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>9</v>
@@ -1017,7 +1017,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>9</v>
@@ -1034,40 +1034,43 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="24.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C2" s="11">
         <v>2</v>
@@ -1080,10 +1083,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="C3" s="11">
         <v>2</v>
@@ -1096,10 +1099,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C4" s="11">
         <v>2</v>
@@ -1112,10 +1115,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C5" s="11">
         <v>-1</v>
@@ -1130,10 +1133,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C6" s="11">
         <v>-1</v>
@@ -1148,10 +1151,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="E7">
         <v>-1</v>
@@ -1169,8 +1172,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
+      <c r="A9" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
@@ -1216,10 +1219,10 @@
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>14</v>
@@ -1245,7 +1248,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -1280,7 +1283,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -1315,7 +1318,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
@@ -1350,7 +1353,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -1385,7 +1388,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -1420,7 +1423,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
@@ -1455,7 +1458,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
@@ -1490,7 +1493,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
@@ -1525,7 +1528,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
@@ -1560,7 +1563,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
@@ -1595,7 +1598,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -1630,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
@@ -1665,7 +1668,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
@@ -1700,7 +1703,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
         <v>20</v>
@@ -1735,7 +1738,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
         <v>20</v>
@@ -1770,7 +1773,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -1805,7 +1808,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
         <v>19</v>
@@ -1877,7 +1880,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B9"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1888,15 +1891,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>4.5</v>
@@ -1904,7 +1907,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1912,7 +1915,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <v>4.5</v>
@@ -1920,7 +1923,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B5">
         <v>0.5</v>
@@ -1928,7 +1931,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B6">
         <v>11</v>
@@ -1936,7 +1939,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B7">
         <v>0.5</v>
@@ -1944,7 +1947,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B8">
         <v>4.5</v>
@@ -1952,7 +1955,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -1960,7 +1963,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B10">
         <v>10</v>
@@ -1968,7 +1971,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B11">
         <v>0.5</v>

</xml_diff>